<commit_message>
Couple more small changes
</commit_message>
<xml_diff>
--- a/Documentation/Updated Feature Backlog.xlsx
+++ b/Documentation/Updated Feature Backlog.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
   <si>
     <t>Stories</t>
   </si>
@@ -247,6 +247,9 @@
     <t>Game Description Page GUI</t>
   </si>
   <si>
+    <t>Usernames Stored and Retrieved from File</t>
+  </si>
+  <si>
     <t>Calculate Score</t>
   </si>
   <si>
@@ -268,13 +271,7 @@
     <t>8,9,13</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Needs Integration</t>
-  </si>
-  <si>
-    <t>Usernames Stored Retrieved from File</t>
   </si>
   <si>
     <t>Enter Username (For Playing Against Computer) Page GUI</t>
@@ -1000,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1195,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C11" s="28">
         <v>2</v>
@@ -1351,7 +1348,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C17" s="29">
         <v>2</v>
@@ -1400,7 +1397,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" s="11">
         <v>2</v>
@@ -1553,13 +1550,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="11">
         <v>2</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>81</v>
@@ -1585,7 +1582,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>29</v>
@@ -1625,7 +1622,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C29" s="23">
         <v>3</v>
@@ -1700,7 +1697,7 @@
         <v>3</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E32" s="30" t="s">
         <v>30</v>
@@ -1740,7 +1737,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="23">
         <v>3</v>
@@ -1775,7 +1772,7 @@
         <v>63</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="F35" s="23">
         <v>2</v>

</xml_diff>